<commit_message>
Merged subarna'sVersion.sql, corrected errors and finished table creation for left side of E-R Diagram
</commit_message>
<xml_diff>
--- a/project_specs.xlsx
+++ b/project_specs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbjkhadka\Desktop\SecondSemester\COMP122\term_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E33E810-0CEA-4C77-88D7-B88C13FB9077}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083AC71D-C91C-424D-B275-EC2956AF4105}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F39D39F4-9C11-42D5-A035-030FBEAA875A}"/>
+    <workbookView xWindow="270" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{F39D39F4-9C11-42D5-A035-030FBEAA875A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>LOCATION ID</t>
   </si>
@@ -39,13 +39,19 @@
     <t>PRODUCT ID</t>
   </si>
   <si>
-    <t>CANPOST</t>
+    <t>EMPLOYEE_ID</t>
   </si>
   <si>
-    <t>Purolator</t>
+    <t>PO_ID</t>
   </si>
   <si>
-    <t>FedEX</t>
+    <t>CUST_id</t>
+  </si>
+  <si>
+    <t>order_id</t>
+  </si>
+  <si>
+    <t>shipper_id</t>
   </si>
 </sst>
 </file>
@@ -68,13 +74,14 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color rgb="FF404040"/>
-      <name val="Segoe UI"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,8 +100,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -117,22 +142,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFF0F0F0"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFF0F0F0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFF0F0F0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF0F0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -140,8 +183,37 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -457,325 +529,546 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{557C324D-0338-49DA-9703-B3432ADE1202}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="M1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="4"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="9"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15">
         <v>10011</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="15">
         <v>20021</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="16">
         <v>30031</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="16">
         <v>40041</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="16">
         <v>50051</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="16">
         <v>60061</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="G3" s="16">
+        <v>70071</v>
+      </c>
+      <c r="H3" s="16">
+        <v>80031</v>
+      </c>
+      <c r="I3" s="13">
+        <v>1</v>
+      </c>
+      <c r="J3" s="14">
+        <v>10</v>
+      </c>
+      <c r="K3" s="14">
+        <v>19</v>
+      </c>
+      <c r="M3" s="10">
+        <v>1001</v>
+      </c>
+      <c r="P3" s="8">
+        <v>1010</v>
+      </c>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="9">
+        <v>1001</v>
+      </c>
+      <c r="S3" s="7">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15">
         <v>10012</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="16">
         <v>20022</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="16">
         <v>30032</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="16">
         <v>40042</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="16">
         <v>50052</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="16">
         <v>60062</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="G4" s="16">
+        <v>70072</v>
+      </c>
+      <c r="H4" s="16">
+        <v>80032</v>
+      </c>
+      <c r="I4" s="13">
+        <v>2</v>
+      </c>
+      <c r="J4" s="14">
+        <v>11</v>
+      </c>
+      <c r="K4" s="14">
+        <v>20</v>
+      </c>
+      <c r="M4" s="10">
+        <v>1002</v>
+      </c>
+      <c r="P4" s="8">
+        <v>1011</v>
+      </c>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="9">
+        <v>1002</v>
+      </c>
+      <c r="S4" s="7">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15">
         <v>10013</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="16">
         <v>20023</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="16">
         <v>30033</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="16">
         <v>40043</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="16">
         <v>50053</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="16">
         <v>60063</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="G5" s="16">
+        <v>70073</v>
+      </c>
+      <c r="H5" s="16">
+        <v>80033</v>
+      </c>
+      <c r="I5" s="13">
+        <v>3</v>
+      </c>
+      <c r="J5" s="14">
+        <v>12</v>
+      </c>
+      <c r="K5" s="14">
+        <v>21</v>
+      </c>
+      <c r="M5" s="10">
+        <v>1003</v>
+      </c>
+      <c r="P5" s="8">
+        <v>2020</v>
+      </c>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="9">
+        <v>1003</v>
+      </c>
+      <c r="S5" s="7">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15">
         <v>10014</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="16">
         <v>20024</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="16">
         <v>30034</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="16">
         <v>40044</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="16">
         <v>50054</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="16">
         <v>60064</v>
       </c>
-      <c r="J6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="G6" s="16">
+        <v>70074</v>
+      </c>
+      <c r="H6" s="16">
+        <v>80034</v>
+      </c>
+      <c r="I6" s="13">
+        <v>4</v>
+      </c>
+      <c r="J6" s="14">
+        <v>13</v>
+      </c>
+      <c r="K6" s="14">
+        <v>22</v>
+      </c>
+      <c r="M6" s="10">
+        <v>1004</v>
+      </c>
+      <c r="P6" s="8">
+        <v>3030</v>
+      </c>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="9">
+        <v>1004</v>
+      </c>
+      <c r="S6" s="7">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15">
         <v>10015</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="16">
         <v>20025</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="16">
         <v>30035</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="16">
         <v>40045</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="16">
         <v>50055</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="16">
         <v>60065</v>
       </c>
-      <c r="J7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="G7" s="16">
+        <v>70075</v>
+      </c>
+      <c r="H7" s="16">
+        <v>80035</v>
+      </c>
+      <c r="I7" s="13">
+        <v>5</v>
+      </c>
+      <c r="J7" s="14">
+        <v>14</v>
+      </c>
+      <c r="K7" s="14">
+        <v>23</v>
+      </c>
+      <c r="M7" s="10">
+        <v>1005</v>
+      </c>
+      <c r="P7" s="8">
+        <v>4040</v>
+      </c>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="9">
+        <v>1005</v>
+      </c>
+      <c r="S7" s="7">
+        <v>4040</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15">
         <v>10016</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="16">
         <v>20026</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="16">
         <v>30036</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="16">
         <v>40046</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="16">
         <v>50056</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="J8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="F8" s="16">
+        <v>60066</v>
+      </c>
+      <c r="G8" s="16">
+        <v>70076</v>
+      </c>
+      <c r="H8" s="16">
+        <v>80036</v>
+      </c>
+      <c r="I8" s="13">
+        <v>6</v>
+      </c>
+      <c r="J8" s="14">
+        <v>15</v>
+      </c>
+      <c r="K8" s="14">
+        <v>24</v>
+      </c>
+      <c r="M8" s="10">
+        <v>1006</v>
+      </c>
+      <c r="P8" s="8">
+        <v>5050</v>
+      </c>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="9">
+        <v>1006</v>
+      </c>
+      <c r="S8" s="7">
+        <v>5050</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
         <v>10017</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="16">
         <v>20027</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="16">
         <v>30037</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="16">
         <v>40047</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="16">
         <v>50057</v>
       </c>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="F9" s="16">
+        <v>60067</v>
+      </c>
+      <c r="G9" s="16">
+        <v>70077</v>
+      </c>
+      <c r="H9" s="16">
+        <v>80037</v>
+      </c>
+      <c r="I9" s="13">
+        <v>7</v>
+      </c>
+      <c r="J9" s="14">
+        <v>16</v>
+      </c>
+      <c r="K9" s="14">
+        <v>25</v>
+      </c>
+      <c r="M9" s="10">
+        <v>1007</v>
+      </c>
+      <c r="P9" s="8">
+        <v>6060</v>
+      </c>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="9">
+        <v>1007</v>
+      </c>
+      <c r="S9" s="7">
+        <v>6060</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15">
         <v>10018</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="16">
         <v>20028</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="16">
         <v>30038</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="16">
         <v>40048</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="16">
         <v>50058</v>
       </c>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="F10" s="16">
+        <v>60068</v>
+      </c>
+      <c r="G10" s="16">
+        <v>70078</v>
+      </c>
+      <c r="H10" s="16">
+        <v>80038</v>
+      </c>
+      <c r="I10" s="13">
+        <v>8</v>
+      </c>
+      <c r="J10" s="14">
+        <v>17</v>
+      </c>
+      <c r="K10" s="14">
+        <v>26</v>
+      </c>
+      <c r="M10" s="10">
+        <v>1008</v>
+      </c>
+      <c r="P10" s="8">
+        <v>7070</v>
+      </c>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="9">
+        <v>1008</v>
+      </c>
+      <c r="S10" s="7">
+        <v>7070</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15">
         <v>10019</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="16">
         <v>20029</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="16">
         <v>30039</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="16">
         <v>40049</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="16">
         <v>50059</v>
       </c>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>1</v>
-      </c>
-      <c r="B16" s="2">
-        <v>10</v>
-      </c>
-      <c r="C16" s="2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>2</v>
-      </c>
-      <c r="B17" s="1">
-        <v>11</v>
-      </c>
-      <c r="C17" s="1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>3</v>
-      </c>
-      <c r="B18" s="2">
-        <v>12</v>
-      </c>
-      <c r="C18" s="2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1">
-        <v>13</v>
-      </c>
-      <c r="C19" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>5</v>
-      </c>
-      <c r="B20" s="2">
-        <v>14</v>
-      </c>
-      <c r="C20" s="2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="F11" s="16">
+        <v>60069</v>
+      </c>
+      <c r="G11" s="16">
+        <v>70079</v>
+      </c>
+      <c r="H11" s="16">
+        <v>80039</v>
+      </c>
+      <c r="I11" s="13">
+        <v>9</v>
+      </c>
+      <c r="J11" s="14">
+        <v>18</v>
+      </c>
+      <c r="K11" s="14">
+        <v>27</v>
+      </c>
+      <c r="M11" s="10">
+        <v>1009</v>
+      </c>
+      <c r="P11" s="8">
+        <v>8080</v>
+      </c>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="9">
+        <v>1009</v>
+      </c>
+      <c r="S11" s="7">
+        <v>8080</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="2"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="3"/>
+      <c r="K12" s="11"/>
+      <c r="M12" s="10">
+        <v>1010</v>
+      </c>
+      <c r="P12" s="8">
+        <v>9090</v>
+      </c>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="9">
+        <v>1010</v>
+      </c>
+      <c r="S12" s="7">
+        <v>9090</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="1">
-        <v>15</v>
-      </c>
-      <c r="C21" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>7</v>
-      </c>
-      <c r="B22" s="2">
-        <v>16</v>
-      </c>
-      <c r="C22" s="2">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>8</v>
-      </c>
-      <c r="B23" s="1">
-        <v>17</v>
-      </c>
-      <c r="C23" s="1">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>9</v>
-      </c>
-      <c r="C24" s="2">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="1">
-        <v>30</v>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="7">
+        <v>10001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="7">
+        <v>10002</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="7">
+        <v>10003</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="7">
+        <v>10004</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="7">
+        <v>10005</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A14:C14"/>
+  <mergeCells count="4">
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>